<commit_message>
logic added to wait for Inquiry updates from IM
</commit_message>
<xml_diff>
--- a/MyProject/sources/drv.xlsx
+++ b/MyProject/sources/drv.xlsx
@@ -4,66 +4,151 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="13395" windowHeight="4170"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="16590" windowHeight="7320"/>
   </bookViews>
   <sheets>
     <sheet name="env" sheetId="2" r:id="rId1"/>
-    <sheet name="TC1" sheetId="1" r:id="rId2"/>
-    <sheet name="TC2" sheetId="3" r:id="rId3"/>
+    <sheet name="SetPersonalSettings" sheetId="3" r:id="rId2"/>
+    <sheet name="MessageBoard" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:O33"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="44">
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>http://153.112.61.197/vss_connect_testr1/Login/Login.aspx?nextview=Welcome</t>
+  </si>
+  <si>
+    <t>webdriver</t>
+  </si>
+  <si>
+    <t>driverlocation</t>
+  </si>
+  <si>
+    <t>webdriver.chrome.driver</t>
+  </si>
+  <si>
+    <t>C:\\Eclipse\\chromedriver.exe</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>brand</t>
+  </si>
+  <si>
+    <t>TYP40US</t>
+  </si>
+  <si>
+    <t>Mack</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>go2personalsettings</t>
+  </si>
+  <si>
+    <t>setru</t>
+  </si>
+  <si>
+    <t>save</t>
+  </si>
+  <si>
+    <t>Test ID</t>
+  </si>
+  <si>
+    <t>Sequence</t>
+  </si>
+  <si>
+    <t>Save the selected RU settings from personal page.</t>
+  </si>
+  <si>
+    <t>Switch to personal setting page via landing page.</t>
+  </si>
+  <si>
+    <t>Select required dealer hood from RU dropdown list.</t>
+  </si>
+  <si>
+    <t>Element</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>moveToElement</t>
+  </si>
+  <si>
+    <t>UC560</t>
+  </si>
+  <si>
+    <t>Sub step 1 Switch to personal setting page via landing page.</t>
+  </si>
+  <si>
+    <t>Sub step 2 Switch to personal setting page via landing page.</t>
+  </si>
+  <si>
+    <t>contentFrame</t>
+  </si>
+  <si>
+    <t>switchTo</t>
+  </si>
   <si>
     <t>Type</t>
   </si>
   <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>Action</t>
-  </si>
-  <si>
-    <t>Login</t>
-  </si>
-  <si>
-    <t>log</t>
-  </si>
-  <si>
-    <t>v0cn140</t>
-  </si>
-  <si>
-    <t>url</t>
-  </si>
-  <si>
-    <t>http://153.112.61.197/vss_connect_testr1/Login/Login.aspx?nextview=Welcome</t>
-  </si>
-  <si>
-    <t>webdriver</t>
-  </si>
-  <si>
-    <t>driverlocation</t>
-  </si>
-  <si>
-    <t>webdriver.chrome.driver</t>
-  </si>
-  <si>
-    <t>C:\\Eclipse\\chromedriver.exe</t>
-  </si>
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>brand</t>
-  </si>
-  <si>
-    <t>TYP40US</t>
-  </si>
-  <si>
-    <t>Mack</t>
+    <t>id</t>
+  </si>
+  <si>
+    <t>xpath</t>
+  </si>
+  <si>
+    <t>PageHeaderTopNavigationMenu_11</t>
+  </si>
+  <si>
+    <t>//tr[@id='PageHeaderTopNavigationMenu_11_3']</t>
+  </si>
+  <si>
+    <t>frame</t>
+  </si>
+  <si>
+    <t>DefaultOrganisationDropDown</t>
+  </si>
+  <si>
+    <t>Select</t>
+  </si>
+  <si>
+    <t>selectByVisibleText</t>
+  </si>
+  <si>
+    <t>Assertion Expected</t>
+  </si>
+  <si>
+    <t>Assertion Actual</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>SaveButton</t>
+  </si>
+  <si>
+    <t>click</t>
+  </si>
+  <si>
+    <t>getFirstSelectedOption</t>
+  </si>
+  <si>
+    <t xml:space="preserve">999425, NEXTRAN CORPORATION - JACKSONVILLE, </t>
   </si>
 </sst>
 </file>
@@ -129,11 +214,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -438,8 +538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,42 +550,42 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -495,51 +595,338 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J15"/>
+    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="60.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="58.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="54.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="3"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="5">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="5">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="5">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="5">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="5">
         <v>5</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="5">
+        <v>6</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="5">
+        <v>7</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="5">
+        <v>8</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>100</v>
+      </c>
+      <c r="B2" s="5">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>100</v>
+      </c>
+      <c r="B3" s="5">
+        <v>2</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>100</v>
+      </c>
+      <c r="B4" s="5">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>